<commit_message>
Ellenség és hátterek beállítása
Ellenség beállítása, karakterválasztás háttérképének beállítása.
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
@@ -631,9 +631,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0" rightToLeft="false">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <col min="4" max="4" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -671,7 +671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -699,7 +699,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -713,7 +713,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="6">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -727,7 +727,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -741,7 +741,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -755,7 +755,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="9">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -769,7 +769,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -783,7 +783,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="11">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -797,7 +797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -811,7 +811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="13">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -825,7 +825,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="14">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -839,7 +839,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="15">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -853,7 +853,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="16">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -867,7 +867,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="17">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -881,7 +881,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="18">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -895,7 +895,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="19">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -909,7 +909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="20">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -923,7 +923,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -937,7 +937,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="22">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
@@ -951,7 +951,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -965,7 +965,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="24">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -979,7 +979,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="25">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -993,7 +993,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="27">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="28">
       <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="29">
       <c r="A29" s="1" t="s">
         <v>86</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="30">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="31">
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
@@ -1075,6 +1075,50 @@
       </c>
       <c r="D31" s="1" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>sfdf</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Harcos</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>csatabárd</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/harcos0.png</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>fdfd</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Harcos</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>lándzsa</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/harcos0.png</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1084,9 +1128,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0" rightToLeft="false">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1096,7 +1140,7 @@
     <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1154,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1124,7 +1168,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1182,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1152,7 +1196,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="5">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1166,7 +1210,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1180,7 +1224,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="7">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1194,7 +1238,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="8">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1208,7 +1252,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="9">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1222,7 +1266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="10">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1236,7 +1280,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="11">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1250,7 +1294,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="12">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1264,7 +1308,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="13">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1278,7 +1322,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="14">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1292,7 +1336,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="15">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1306,7 +1350,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="16">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1364,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="17">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1334,7 +1378,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="18">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1348,7 +1392,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="19">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1362,7 +1406,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="20">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1376,7 +1420,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="21">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1434,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="22">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1404,7 +1448,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="23">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1418,7 +1462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="24">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1432,7 +1476,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="25">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1446,7 +1490,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -1460,7 +1504,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="27">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -1474,7 +1518,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row spans="1:4" outlineLevel="0" r="28">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
@@ -1486,6 +1530,28 @@
       </c>
       <c r="D28" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>hghdgssdf</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Mágus</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>tűz botja</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/magus1.png</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GlobalClass osztály létrehozása, a Betoltes Window kidolgozása
- Betöltés window-on belül, az első ComboBox tartalmazza a kasztok
nevét, ha a mellette levő kiválasztra kattintunk, akkor az alatta levő
ComboBox feltöltődik azokkal a korábbi játékos nevekkel, amiknek a
kasztja a kiválasztott kaszt volt. Ezután a második kiválasztra
kattintva a program átirányít a Harcter Windowra.
- GlobalClass osztály feladata, hogy eltárolja a betölteni kívánt
karakter adatait, hogy a Harcter Window-on belül is hozzáférhessünk.
// Fennálló hiba:  - Jelenleg a betölteni kívánt karakterhez nem
mentettük le korábban a kiválasztott fegyverét, ezért a betöltés után a
harctérre érkezve hibát dob fel, a létrehozása és a betöltése
átalakításra szorul. //
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
@@ -1150,7 +1150,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0" rightToLeft="false">
       <selection activeCell="E26" sqref="E26"/>
@@ -1615,6 +1615,28 @@
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/magus1.png</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>etzui</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Mágus</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>föld botja</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
         <is>
           <t>/Images/Karakterek/magus1.png</t>
         </is>

</xml_diff>

<commit_message>
Betoltes Window hibájának javítása
- A régebben létrehozott karakterek betöltése működik mindegyik kaszt
esetében, a korábbi hiba javítva.
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
@@ -631,7 +631,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0" rightToLeft="false">
       <selection activeCell="D31" sqref="D31"/>
@@ -1165,6 +1165,28 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>tzuiopő</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>Harcos</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>katana</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/harcos1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1172,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0" rightToLeft="false">
       <selection activeCell="E26" sqref="E26"/>
@@ -1659,6 +1681,28 @@
         </is>
       </c>
       <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/magus1.png</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Uiorepzr</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Mágus</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>szél botja</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
         <is>
           <t>/Images/Karakterek/magus1.png</t>
         </is>

</xml_diff>

<commit_message>
Következő ellenfél button használhatóságának korrigálása
- vesztes csata után a Következő ellenfél gombra kattintva egy
MessageBox ugrik fel egy figyelmeztető üzenettel, hogy a harcot
elveszítettük, így nem küzdhetünk egy újabb ellenség ellen.
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/jatekosadatbazis.xlsx
@@ -1194,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0" rightToLeft="false">
       <selection activeCell="E26" sqref="E26"/>
@@ -1705,6 +1705,28 @@
       <c r="D33" s="1" t="inlineStr">
         <is>
           <t>/Images/Karakterek/magus1.png</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>krjthznfnf</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>Mágus</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>éjtalizmán</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="inlineStr">
+        <is>
+          <t>/Images/Karakterek/magus0.png</t>
         </is>
       </c>
     </row>

</xml_diff>